<commit_message>
Update to use 5V for consistent ATTINY20 programming
</commit_message>
<xml_diff>
--- a/pcb/ird-v17 bom.xlsx
+++ b/pcb/ird-v17 bom.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects-Electronics\ir-detector\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD23E7FA-2CDC-434E-9F1D-EC9EF96D3AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C326A8-E2B2-4ECF-9C02-597D77890F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5ADBABA9-B6A2-4FDA-A94D-E4ECFBA9FE86}"/>
   </bookViews>
   <sheets>
     <sheet name="ird-v17 bom" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t>Value</t>
   </si>
@@ -106,9 +119,6 @@
     <t>K1</t>
   </si>
   <si>
-    <t>G6K-2G-Y-TR DC3</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -127,21 +137,9 @@
     <t>R2</t>
   </si>
   <si>
-    <t>27R</t>
-  </si>
-  <si>
-    <t>RCS040227R0FKED</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
-    <t>120R</t>
-  </si>
-  <si>
-    <t>RCS0402120RFKED</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -154,15 +152,9 @@
     <t>U3</t>
   </si>
   <si>
-    <t>TLVM365R15RDNR</t>
-  </si>
-  <si>
     <t>VR1</t>
   </si>
   <si>
-    <t>TC42X-2-10E</t>
-  </si>
-  <si>
     <t>2.2µF</t>
   </si>
   <si>
@@ -193,9 +185,6 @@
     <t>NPN 10K 10K x2</t>
   </si>
   <si>
-    <t>3.3V</t>
-  </si>
-  <si>
     <t>860020575016</t>
   </si>
   <si>
@@ -230,6 +219,33 @@
   </si>
   <si>
     <t>Ref</t>
+  </si>
+  <si>
+    <t>G6K-2G-Y-TR DC5</t>
+  </si>
+  <si>
+    <t>RCS0402750RFKED</t>
+  </si>
+  <si>
+    <t>750R</t>
+  </si>
+  <si>
+    <t>56R</t>
+  </si>
+  <si>
+    <t>RCS040256R0FKED</t>
+  </si>
+  <si>
+    <t>TLVM365R1RDNR</t>
+  </si>
+  <si>
+    <t>IR Detector</t>
+  </si>
+  <si>
+    <t>5V SMPS</t>
+  </si>
+  <si>
+    <t>TC42X-2-103E</t>
   </si>
 </sst>
 </file>
@@ -816,11 +832,11 @@
     <tableColumn id="2" xr3:uid="{B9ED98D1-0381-4254-8FBE-E7184FABF976}" name="Value"/>
     <tableColumn id="3" xr3:uid="{3B98DFDF-B559-4E29-9A21-D8FC6877A58D}" name="SKU" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{3D4F99BD-BA55-42CC-A0A3-EA54B55502D3}" name="Status"/>
-    <tableColumn id="7" xr3:uid="{63E1CABB-5B1C-4B97-80D8-F957570A34EB}" name="$/1" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{2318C61F-E61C-4238-B39C-82E206D1EA18}" name="$/3" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="1">
+    <tableColumn id="7" xr3:uid="{63E1CABB-5B1C-4B97-80D8-F957570A34EB}" name="$/1" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{2318C61F-E61C-4238-B39C-82E206D1EA18}" name="$/3" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="1">
       <calculatedColumnFormula>3*E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{989EB49D-B317-4905-9835-73B83EDA5CF1}" name="$/10" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{989EB49D-B317-4905-9835-73B83EDA5CF1}" name="$/10" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1146,7 +1162,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,22 +1175,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1185,7 +1201,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -1227,7 +1243,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
@@ -1248,7 +1264,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
@@ -1290,10 +1306,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E7" s="1">
         <v>0.61</v>
@@ -1311,7 +1327,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>16</v>
@@ -1332,7 +1348,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>18</v>
@@ -1353,7 +1369,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>20</v>
@@ -1380,7 +1396,7 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E11" s="1">
         <v>0.44</v>
@@ -1398,7 +1414,7 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>25</v>
@@ -1422,10 +1438,10 @@
         <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E13" s="1">
         <v>0.81</v>
@@ -1443,31 +1459,31 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="E14" s="1">
-        <v>4.3</v>
+        <v>4.21</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>12.899999999999999</v>
+        <v>12.629999999999999</v>
       </c>
       <c r="G14" s="1">
-        <v>38.28</v>
+        <v>39.79</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="E15" s="1">
         <v>0.23</v>
@@ -1482,13 +1498,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="E16" s="1">
         <v>0.11</v>
@@ -1503,13 +1519,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="E17" s="1">
         <v>0.12</v>
@@ -1519,42 +1535,42 @@
         <v>0.36</v>
       </c>
       <c r="G17" s="1">
-        <v>0.54</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E18" s="1">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>0.33</v>
+        <v>0.36</v>
       </c>
       <c r="G18" s="1">
-        <v>0.53</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E19" s="1">
         <v>1.18</v>
@@ -1569,13 +1585,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E20" s="1">
         <v>1.34</v>
@@ -1590,34 +1606,34 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="E21" s="1">
-        <v>2.4</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>7.1999999999999993</v>
+        <v>6.84</v>
       </c>
       <c r="G21" s="1">
-        <v>17.79</v>
+        <v>16.87</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="E22" s="1">
         <v>0.45</v>
@@ -1632,16 +1648,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E23" s="1">
         <v>2</v>
@@ -1656,19 +1672,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E24" s="1">
         <f>SUBTOTAL(109,Table1[$/1])</f>
-        <v>16.79</v>
+        <v>16.589999999999996</v>
       </c>
       <c r="F24" s="1">
         <f>SUBTOTAL(109,Table1[$/3])</f>
-        <v>50.37</v>
+        <v>49.77</v>
       </c>
       <c r="G24" s="1">
         <f>SUBTOTAL(109,Table1[$/10])</f>
-        <v>139.38999999999999</v>
+        <v>140.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>